<commit_message>
Update Compiled 2008-2020 UCUES Data.xlsx
</commit_message>
<xml_diff>
--- a/sources/Compiled 2008-2020 UCUES Data.xlsx
+++ b/sources/Compiled 2008-2020 UCUES Data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thepe\Documents\GitHub\pride\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thepe\Documents\GitHub\campus-pride\sources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA84C269-D952-4D15-9FBC-92092FEF716D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FF774DC-59A6-46A8-97C4-E57FA898BFFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20220" yWindow="10430" windowWidth="10160" windowHeight="5640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19090" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -296,7 +296,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -328,10 +328,16 @@
     <xf numFmtId="164" fontId="3" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -340,18 +346,14 @@
     <xf numFmtId="9" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="3" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -669,8 +671,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A3:S40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="S18" sqref="S18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -684,92 +686,92 @@
   <sheetData>
     <row r="3" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A3" s="10"/>
-      <c r="B3" s="33">
+      <c r="B3" s="27">
         <v>2008</v>
       </c>
-      <c r="C3" s="34"/>
-      <c r="D3" s="31">
+      <c r="C3" s="28"/>
+      <c r="D3" s="29">
         <v>2009</v>
       </c>
-      <c r="E3" s="32"/>
-      <c r="F3" s="33">
+      <c r="E3" s="30"/>
+      <c r="F3" s="27">
         <v>2010</v>
       </c>
-      <c r="G3" s="34"/>
-      <c r="H3" s="31">
+      <c r="G3" s="28"/>
+      <c r="H3" s="29">
         <v>2011</v>
       </c>
-      <c r="I3" s="32"/>
-      <c r="J3" s="33">
+      <c r="I3" s="30"/>
+      <c r="J3" s="27">
         <v>2012</v>
       </c>
-      <c r="K3" s="34"/>
-      <c r="L3" s="31">
+      <c r="K3" s="28"/>
+      <c r="L3" s="29">
         <v>2014</v>
       </c>
-      <c r="M3" s="32"/>
-      <c r="N3" s="33">
+      <c r="M3" s="30"/>
+      <c r="N3" s="27">
         <v>2016</v>
       </c>
-      <c r="O3" s="34"/>
-      <c r="P3" s="31">
+      <c r="O3" s="28"/>
+      <c r="P3" s="29">
         <v>2018</v>
       </c>
-      <c r="Q3" s="32"/>
-      <c r="R3" s="33">
+      <c r="Q3" s="30"/>
+      <c r="R3" s="27">
         <v>2020</v>
       </c>
-      <c r="S3" s="34"/>
+      <c r="S3" s="28"/>
     </row>
     <row r="4" spans="1:19" s="17" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="27">
+      <c r="B4" s="33">
         <f>11833/23904</f>
         <v>0.49502175368139223</v>
       </c>
-      <c r="C4" s="28"/>
-      <c r="D4" s="29">
+      <c r="C4" s="34"/>
+      <c r="D4" s="31">
         <f>9016/24379</f>
         <v>0.36982649001189549</v>
       </c>
-      <c r="E4" s="30"/>
-      <c r="F4" s="27">
+      <c r="E4" s="32"/>
+      <c r="F4" s="33">
         <f>11203/24967</f>
         <v>0.44871230023631192</v>
       </c>
-      <c r="G4" s="28"/>
-      <c r="H4" s="29">
+      <c r="G4" s="34"/>
+      <c r="H4" s="31">
         <f>6982/23656</f>
         <v>0.29514710855596887</v>
       </c>
-      <c r="I4" s="30"/>
-      <c r="J4" s="27">
+      <c r="I4" s="32"/>
+      <c r="J4" s="33">
         <f>8209/25203</f>
         <v>0.32571519263579735</v>
       </c>
-      <c r="K4" s="28"/>
-      <c r="L4" s="29">
+      <c r="K4" s="34"/>
+      <c r="L4" s="31">
         <f>8019/25402</f>
         <v>0.31568380442484845</v>
       </c>
-      <c r="M4" s="30"/>
-      <c r="N4" s="27">
+      <c r="M4" s="32"/>
+      <c r="N4" s="33">
         <f>7515/26027</f>
         <v>0.28873861758942637</v>
       </c>
-      <c r="O4" s="28"/>
-      <c r="P4" s="29">
+      <c r="O4" s="34"/>
+      <c r="P4" s="31">
         <f>9944/28918</f>
         <v>0.34386887059962651</v>
       </c>
-      <c r="Q4" s="30"/>
-      <c r="R4" s="27">
+      <c r="Q4" s="32"/>
+      <c r="R4" s="33">
         <f>11390/29459</f>
         <v>0.38663905767337658</v>
       </c>
-      <c r="S4" s="28"/>
+      <c r="S4" s="34"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A5" s="9" t="s">
@@ -991,10 +993,10 @@
         <f t="shared" si="2"/>
         <v>0.85421858312566745</v>
       </c>
-      <c r="H8" s="14">
+      <c r="H8" s="35">
         <v>5955</v>
       </c>
-      <c r="I8" s="24">
+      <c r="I8" s="36">
         <f t="shared" si="3"/>
         <v>0.85229712322885354</v>
       </c>
@@ -2033,25 +2035,25 @@
         <v>0.57789123723581093</v>
       </c>
       <c r="N23" s="1">
-        <v>2987</v>
+        <v>4470</v>
       </c>
       <c r="O23" s="2">
-        <f t="shared" ref="O23:O28" si="26">N23/N$29</f>
-        <v>0.3925614403995269</v>
+        <f t="shared" ref="O23:Q24" si="26">N23/N$29</f>
+        <v>0.58746221579708235</v>
       </c>
       <c r="P23" s="12">
-        <v>4080</v>
+        <v>5712</v>
       </c>
       <c r="Q23" s="13">
-        <f t="shared" ref="Q23:Q28" si="27">P23/P$29</f>
-        <v>0.40779610194902549</v>
+        <f t="shared" si="26"/>
+        <v>0.57091454272863573</v>
       </c>
       <c r="R23" s="1">
-        <v>4480</v>
+        <v>6912</v>
       </c>
       <c r="S23" s="2">
-        <f t="shared" ref="S23:S28" si="28">R23/R$29</f>
-        <v>0.38398902888488901</v>
+        <f t="shared" ref="S23" si="27">R23/R$29</f>
+        <v>0.59244021599382879</v>
       </c>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.35">
@@ -2101,25 +2103,25 @@
         <v>0.39658038470672047</v>
       </c>
       <c r="N24" s="1">
-        <v>4470</v>
+        <v>2987</v>
       </c>
       <c r="O24" s="2">
         <f t="shared" si="26"/>
-        <v>0.58746221579708235</v>
+        <v>0.3925614403995269</v>
       </c>
       <c r="P24" s="12">
-        <v>5712</v>
+        <v>4080</v>
       </c>
       <c r="Q24" s="13">
-        <f t="shared" si="27"/>
-        <v>0.57091454272863573</v>
+        <f t="shared" ref="Q24" si="28">P24/P$29</f>
+        <v>0.40779610194902549</v>
       </c>
       <c r="R24" s="1">
-        <v>6912</v>
+        <v>4480</v>
       </c>
       <c r="S24" s="2">
-        <f t="shared" si="28"/>
-        <v>0.59244021599382879</v>
+        <f t="shared" ref="S24" si="29">R24/R$29</f>
+        <v>0.38398902888488901</v>
       </c>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.35">
@@ -2172,7 +2174,7 @@
         <v>21</v>
       </c>
       <c r="O25" s="2">
-        <f t="shared" si="26"/>
+        <f t="shared" ref="O23:O28" si="30">N25/N$29</f>
         <v>2.7598896044158236E-3</v>
       </c>
       <c r="P25" s="12">
@@ -2180,7 +2182,7 @@
         <v>29</v>
       </c>
       <c r="Q25" s="13">
-        <f t="shared" si="27"/>
+        <f t="shared" ref="Q23:Q28" si="31">P25/P$29</f>
         <v>2.8985507246376812E-3</v>
       </c>
       <c r="R25" s="1">
@@ -2188,7 +2190,7 @@
         <v>34</v>
       </c>
       <c r="S25" s="2">
-        <f t="shared" si="28"/>
+        <f t="shared" ref="S23:S28" si="32">R25/R$29</f>
         <v>2.9142024513585324E-3</v>
       </c>
     </row>
@@ -2242,21 +2244,21 @@
         <v>87</v>
       </c>
       <c r="O26" s="2">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>1.1433828361151269E-2</v>
       </c>
       <c r="P26" s="12">
         <v>135</v>
       </c>
       <c r="Q26" s="13">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>1.3493253373313344E-2</v>
       </c>
       <c r="R26" s="1">
         <v>190</v>
       </c>
       <c r="S26" s="2">
-        <f t="shared" si="28"/>
+        <f t="shared" si="32"/>
         <v>1.6285248992885918E-2</v>
       </c>
     </row>
@@ -2310,21 +2312,21 @@
         <v>44</v>
       </c>
       <c r="O27" s="2">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>5.7826258378236295E-3</v>
       </c>
       <c r="P27" s="12">
         <v>49</v>
       </c>
       <c r="Q27" s="13">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>4.8975512243878061E-3</v>
       </c>
       <c r="R27" s="1">
         <v>51</v>
       </c>
       <c r="S27" s="2">
-        <f t="shared" si="28"/>
+        <f t="shared" si="32"/>
         <v>4.3713036770377991E-3</v>
       </c>
     </row>
@@ -2378,21 +2380,21 @@
         <v>0</v>
       </c>
       <c r="O28" s="2">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
       <c r="P28" s="23">
         <v>0</v>
       </c>
       <c r="Q28" s="13">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
       <c r="R28" s="21">
         <v>0</v>
       </c>
       <c r="S28" s="2">
-        <f t="shared" si="28"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
     </row>
@@ -2401,75 +2403,75 @@
         <v>8</v>
       </c>
       <c r="B29" s="6">
-        <f t="shared" ref="B29:S29" si="29">SUM(B23:B28)</f>
+        <f t="shared" ref="B29:M29" si="33">SUM(B23:B28)</f>
         <v>2</v>
       </c>
       <c r="C29" s="7">
-        <f t="shared" si="29"/>
+        <f t="shared" si="33"/>
         <v>1</v>
       </c>
       <c r="D29" s="15">
-        <f t="shared" si="29"/>
+        <f t="shared" si="33"/>
         <v>8814</v>
       </c>
       <c r="E29" s="16">
-        <f t="shared" si="29"/>
+        <f t="shared" si="33"/>
         <v>1</v>
       </c>
       <c r="F29" s="6">
-        <f t="shared" si="29"/>
+        <f t="shared" si="33"/>
         <v>11266</v>
       </c>
       <c r="G29" s="7">
-        <f t="shared" si="29"/>
+        <f t="shared" si="33"/>
         <v>1</v>
       </c>
       <c r="H29" s="15">
-        <f t="shared" si="29"/>
+        <f t="shared" si="33"/>
         <v>7016</v>
       </c>
       <c r="I29" s="16">
-        <f t="shared" si="29"/>
+        <f t="shared" si="33"/>
         <v>1</v>
       </c>
       <c r="J29" s="6">
-        <f t="shared" si="29"/>
+        <f t="shared" si="33"/>
         <v>8334</v>
       </c>
       <c r="K29" s="7">
-        <f t="shared" si="29"/>
+        <f t="shared" si="33"/>
         <v>0.99999999999999989</v>
       </c>
       <c r="L29" s="15">
-        <f t="shared" si="29"/>
+        <f t="shared" si="33"/>
         <v>8422</v>
       </c>
       <c r="M29" s="16">
-        <f t="shared" si="29"/>
+        <f t="shared" si="33"/>
         <v>0.99999999999999989</v>
       </c>
       <c r="N29" s="6">
-        <f t="shared" si="29"/>
+        <f>SUM(N23:N28)</f>
         <v>7609</v>
       </c>
       <c r="O29" s="7">
-        <f t="shared" si="29"/>
+        <f>SUM(O23:O28)</f>
         <v>1</v>
       </c>
       <c r="P29" s="15">
-        <f t="shared" si="29"/>
+        <f>SUM(P23:P28)</f>
         <v>10005</v>
       </c>
       <c r="Q29" s="16">
-        <f t="shared" si="29"/>
+        <f>SUM(Q23:Q28)</f>
         <v>1</v>
       </c>
       <c r="R29" s="6">
-        <f t="shared" si="29"/>
+        <f>SUM(R23:R28)</f>
         <v>11667</v>
       </c>
       <c r="S29" s="7">
-        <f t="shared" si="29"/>
+        <f>SUM(S23:S28)</f>
         <v>1</v>
       </c>
     </row>
@@ -2604,11 +2606,11 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="J4:K4"/>
     <mergeCell ref="L4:M4"/>
     <mergeCell ref="N4:O4"/>
     <mergeCell ref="P4:Q4"/>
@@ -2617,11 +2619,11 @@
     <mergeCell ref="N3:O3"/>
     <mergeCell ref="P3:Q3"/>
     <mergeCell ref="R3:S3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="H3:I3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>